<commit_message>
adding the start of a toolbox for gutting the export format. This toolbox still needs modifications in the ValidatorClass and in the sctipt code altogether - it is more or less a testing toolbox for now
</commit_message>
<xml_diff>
--- a/script/EXPORT_REFORMAT_PREPARATION.xlsx
+++ b/script/EXPORT_REFORMAT_PREPARATION.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="198">
   <si>
     <t>'isSearchable'</t>
   </si>
@@ -620,17 +620,26 @@
     <t>*those in red relate to Export format and should be removed</t>
   </si>
   <si>
-    <t>Comment:</t>
-  </si>
-  <si>
-    <t>We might be best off repurposing this parameter (such as Zoning vs Parcels?)</t>
+    <t>Comments:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentatively repurpose for something (i.e. zoning or parcel submission?) </t>
+  </si>
+  <si>
+    <t>Old Index</t>
+  </si>
+  <si>
+    <t>New Index</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,6 +669,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -681,12 +696,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,26 +983,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="3" max="3" width="71.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
@@ -994,770 +1012,1346 @@
         <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="3">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="3">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="3">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="3">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="3">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="3">
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="3">
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="3">
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="3">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="3">
+        <v>31</v>
+      </c>
+      <c r="D34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C35" s="3">
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C36" s="1">
+        <v>33</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C37" s="1">
+        <v>34</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C38" s="1">
+        <v>35</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="C39" s="1">
+        <v>36</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C40" s="1">
+        <v>37</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C41" s="1">
+        <v>38</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C42" s="1">
+        <v>39</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C43" s="1">
+        <v>40</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C44" s="1">
+        <v>41</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C45" s="1">
+        <v>42</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C46" s="1">
+        <v>43</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C47" s="1">
+        <v>44</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C48" s="1">
+        <v>45</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C49" s="1">
+        <v>46</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C50" s="1">
+        <v>47</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C51" s="1">
+        <v>48</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="C52" s="1">
+        <v>49</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="C53" s="1">
+        <v>50</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="C54" s="1">
+        <v>51</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="C55" s="1">
+        <v>52</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="C56" s="1">
+        <v>53</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="1">
+        <v>54</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="1">
+        <v>55</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="1">
+        <v>56</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="1">
+        <v>57</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="1">
+        <v>58</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="1">
+        <v>59</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="1">
+        <v>60</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="1">
+        <v>61</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="1">
+        <v>62</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="1">
+        <v>63</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>64</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
+        <v>65</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
+        <v>66</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
+        <v>67</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>68</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>69</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>70</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="1">
+        <v>71</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="1">
+        <v>72</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="1">
+        <v>73</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="1">
+        <v>74</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" s="1">
+        <v>75</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="1">
+        <v>76</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" s="1">
+        <v>77</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" s="1">
+        <v>78</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" s="1">
+        <v>79</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" s="1">
+        <v>80</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" s="1">
+        <v>81</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" s="1">
+        <v>82</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" s="1">
+        <v>83</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87" s="1">
+        <v>84</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88" s="1">
+        <v>85</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89" s="1">
+        <v>86</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90" s="1">
+        <v>87</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91" s="1">
+        <v>88</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92" s="1">
+        <v>89</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93" s="1">
+        <v>90</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94" s="1">
+        <v>91</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95" s="1">
+        <v>92</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" s="1">
+        <v>93</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>188</v>
+      </c>
+      <c r="C97" s="1">
+        <v>94</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>